<commit_message>
Added the third scenario - Vin Stub
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSAA\CODE\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw3eraj\projects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>PRODUCTCD</t>
   </si>
@@ -50,9 +50,6 @@
     <t>MSRP_VERSION</t>
   </si>
   <si>
-    <t>SYMBOL_2018</t>
-  </si>
-  <si>
     <t>AAA_CSA</t>
   </si>
   <si>
@@ -60,18 +57,6 @@
   </si>
   <si>
     <t>CA</t>
-  </si>
-  <si>
-    <t>CHOICE</t>
-  </si>
-  <si>
-    <t>SYMBOL_2000_CHOICE</t>
-  </si>
-  <si>
-    <t>MSRP_2000_CHOICE</t>
-  </si>
-  <si>
-    <t>SYMBOL_2018_CHOICE</t>
   </si>
   <si>
     <t>EFFECTIVEDATE</t>
@@ -407,23 +392,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +422,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -446,15 +431,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -463,79 +448,10 @@
         <v>20000101</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>99999999</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>99999999</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>20000101</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>99999999</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing the CA control table update version values
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>PRODUCTCD</t>
   </si>
@@ -44,9 +44,6 @@
     <t>SYMBOL_2000</t>
   </si>
   <si>
-    <t>MSRP_2000</t>
-  </si>
-  <si>
     <t>MSRP_VERSION</t>
   </si>
   <si>
@@ -60,6 +57,12 @@
   </si>
   <si>
     <t>EFFECTIVEDATE</t>
+  </si>
+  <si>
+    <t>SYMBOL_2018</t>
+  </si>
+  <si>
+    <t>MSRP_2000_SELECT</t>
   </si>
 </sst>
 </file>
@@ -82,7 +85,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,8 +97,14 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,14 +112,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -392,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,24 +447,24 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -447,11 +472,34 @@
       <c r="E2">
         <v>20000101</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
+        <v>20190701</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2">
+        <v>20190702</v>
+      </c>
+      <c r="F3">
         <v>99999999</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
+      <c r="G3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>